<commit_message>
autosum & auto fill
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -200,9 +200,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -216,6 +213,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -525,7 +525,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,19 +535,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -580,11 +580,11 @@
         <v>60</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E4" si="0">(C3*D3)</f>
-        <v>60</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -611,11 +611,11 @@
       <c r="C5" s="1"/>
       <c r="D5">
         <f>SUM(D2:D4)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E5">
-        <f>(E2+E3+E4)</f>
-        <v>460</v>
+        <f>SUM(E2:E4)</f>
+        <v>520</v>
       </c>
     </row>
   </sheetData>
@@ -645,198 +645,198 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" spans="3:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>16001</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>0.39583333333333331</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>43466</v>
       </c>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>16002</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>43497</v>
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>16003</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>43525</v>
       </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>16004</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>43556</v>
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>16005</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>0.47916666666666702</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>43586</v>
       </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>16006</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>0.5</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <v>43617</v>
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>16007</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>0.52083333333333304</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>43647</v>
       </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>16008</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <v>43678</v>
       </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>16009</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>0.5625</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <v>43709</v>
       </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>16010</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <v>43738</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="5">
         <v>43739</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some new rules added
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>SI NO.</t>
   </si>
@@ -115,6 +115,18 @@
   </si>
   <si>
     <t>PRICE</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>status</t>
   </si>
 </sst>
 </file>
@@ -150,11 +162,11 @@
       <family val="1"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Britannic Bold"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -178,8 +190,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -192,8 +204,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -212,17 +225,46 @@
     <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="60% - Accent2" xfId="1" builtinId="36"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -522,10 +564,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,24 +576,27 @@
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -561,15 +606,16 @@
       <c r="C2" s="1">
         <v>100</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>3</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="7">
         <f>(C2*D2)</f>
         <v>300</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -579,15 +625,16 @@
       <c r="C3" s="1">
         <v>60</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>2</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E4" si="0">(C3*D3)</f>
+      <c r="E3" s="7">
+        <f>(C3*D3)</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -597,28 +644,69 @@
       <c r="C4" s="1">
         <v>20</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>5</v>
       </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
+      <c r="E4" s="7">
+        <f>(C4*D4)</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5">
+      <c r="D5" s="1">
         <f>SUM(D2:D4)</f>
         <v>10</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="7">
         <f>SUM(E2:E4)</f>
         <v>520</v>
       </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="7">
+        <f>AVERAGE(E2:E5)</f>
+        <v>260</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="7">
+        <f>MIN(E2:E6)</f>
+        <v>100</v>
+      </c>
+      <c r="F7" s="1"/>
     </row>
   </sheetData>
+  <sortState ref="A2:E4">
+    <sortCondition descending="1" ref="E2:E4"/>
+  </sortState>
+  <conditionalFormatting sqref="E2:E7">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+      <formula>310</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>310</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -632,7 +720,7 @@
   <dimension ref="C1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,13 +733,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="3:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">

</xml_diff>